<commit_message>
Added delta growth (calculate new cases)
</commit_message>
<xml_diff>
--- a/src/assets/table.xlsx
+++ b/src/assets/table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
   <si>
     <t>Fälle</t>
   </si>
@@ -602,37 +602,37 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:Z54"/>
+  <dimension ref="A2:AB54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.140625" customWidth="1"/>
-    <col min="2" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1"/>
-    <col min="13" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" customWidth="1"/>
+    <col min="2" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="12" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" customWidth="1"/>
+    <col min="15" max="16" width="11.5703125" customWidth="1"/>
     <col min="17" max="17" width="11.42578125" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" customWidth="1"/>
+    <col min="19" max="19" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="I3" s="9"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>38</v>
       </c>
@@ -711,197 +711,219 @@
       <c r="Z6" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="13">
+        <v>43912</v>
+      </c>
+      <c r="C7" s="13">
+        <v>43911</v>
+      </c>
+      <c r="D7" s="13">
         <v>43910</v>
       </c>
-      <c r="C7" s="13">
+      <c r="E7" s="13">
         <v>43909</v>
       </c>
-      <c r="D7" s="13">
+      <c r="F7" s="13">
         <v>43908</v>
       </c>
-      <c r="E7" s="13">
+      <c r="G7" s="13">
         <v>43907</v>
       </c>
-      <c r="F7" s="12">
+      <c r="H7" s="12">
         <v>43906</v>
       </c>
-      <c r="G7" s="12">
+      <c r="I7" s="12">
         <v>43905</v>
       </c>
-      <c r="H7" s="12">
+      <c r="J7" s="12">
         <v>43904</v>
       </c>
-      <c r="I7" s="12">
+      <c r="K7" s="12">
         <v>43903</v>
       </c>
-      <c r="J7" s="12">
+      <c r="L7" s="12">
         <v>43902</v>
       </c>
-      <c r="K7" s="12">
+      <c r="M7" s="12">
         <v>43901</v>
       </c>
-      <c r="L7" s="12">
+      <c r="N7" s="12">
         <v>43900</v>
       </c>
-      <c r="M7" s="12">
+      <c r="O7" s="12">
         <v>43899</v>
       </c>
-      <c r="N7" s="12">
+      <c r="P7" s="12">
         <v>43898</v>
       </c>
-      <c r="O7" s="12">
+      <c r="Q7" s="12">
         <v>43897</v>
       </c>
-      <c r="P7" s="12">
+      <c r="R7" s="12">
         <v>43896</v>
       </c>
-      <c r="Q7" s="12">
+      <c r="S7" s="12">
         <v>43895</v>
       </c>
-      <c r="R7" s="12">
+      <c r="T7" s="12">
         <v>43894</v>
       </c>
-      <c r="S7" s="12">
+      <c r="U7" s="12">
         <v>43893</v>
       </c>
-      <c r="T7" s="12">
+      <c r="V7" s="12">
         <v>43892</v>
       </c>
-      <c r="U7" s="12">
+      <c r="W7" s="12">
         <v>43891</v>
       </c>
-      <c r="V7" s="12">
+      <c r="X7" s="12">
         <v>43890</v>
       </c>
-      <c r="W7" s="12">
+      <c r="Y7" s="12">
         <v>43889</v>
       </c>
-      <c r="X7" s="12">
+      <c r="Z7" s="12">
         <v>43888</v>
       </c>
-      <c r="Y7" s="12">
+      <c r="AA7" s="12">
         <v>43887</v>
       </c>
-      <c r="Z7" s="12">
+      <c r="AB7" s="12">
         <v>43886</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="4">
+        <v>44</v>
+      </c>
+      <c r="C8" s="4">
         <v>39</v>
       </c>
-      <c r="C8" s="4">
+      <c r="D8" s="4">
+        <v>39</v>
+      </c>
+      <c r="E8" s="4">
         <v>26</v>
       </c>
-      <c r="D8" s="4">
+      <c r="F8" s="4">
         <v>26</v>
       </c>
-      <c r="E8" s="4">
+      <c r="G8" s="4">
         <v>24</v>
       </c>
-      <c r="F8" s="4">
+      <c r="H8" s="4">
         <v>13</v>
       </c>
-      <c r="G8" s="4">
+      <c r="I8" s="4">
         <v>12</v>
       </c>
-      <c r="H8" s="4">
+      <c r="J8" s="4">
         <v>7</v>
       </c>
-      <c r="I8" s="3">
+      <c r="K8" s="3">
         <v>6</v>
       </c>
-      <c r="J8" s="4">
+      <c r="L8" s="4">
         <v>6</v>
       </c>
-      <c r="K8" s="3">
-        <v>4</v>
-      </c>
-      <c r="L8" s="4">
-        <v>3</v>
-      </c>
-      <c r="M8" s="4">
-        <v>3</v>
-      </c>
-      <c r="N8" s="3">
-        <v>3</v>
-      </c>
-      <c r="O8" s="3">
+      <c r="M8" s="3">
+        <v>4</v>
+      </c>
+      <c r="N8" s="4">
+        <v>3</v>
+      </c>
+      <c r="O8" s="4">
         <v>3</v>
       </c>
       <c r="P8" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q8" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R8" s="3">
         <v>2</v>
       </c>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
+      <c r="S8" s="3">
+        <v>2</v>
+      </c>
+      <c r="T8" s="3">
+        <v>2</v>
+      </c>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="4">
+        <v>25</v>
+      </c>
+      <c r="C9" s="4">
         <v>21</v>
       </c>
-      <c r="C9" s="4">
+      <c r="D9" s="4">
+        <v>21</v>
+      </c>
+      <c r="E9" s="4">
         <v>17</v>
       </c>
-      <c r="D9" s="4">
+      <c r="F9" s="4">
         <v>14</v>
       </c>
-      <c r="E9" s="4">
+      <c r="G9" s="4">
         <v>12</v>
       </c>
-      <c r="F9" s="4">
+      <c r="H9" s="4">
         <v>7</v>
       </c>
-      <c r="G9" s="4">
+      <c r="I9" s="4">
         <v>5</v>
       </c>
-      <c r="H9" s="4">
-        <v>4</v>
-      </c>
-      <c r="I9" s="3">
-        <v>3</v>
-      </c>
       <c r="J9" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K9" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L9" s="4">
-        <v>1</v>
-      </c>
-      <c r="M9" s="4">
-        <v>1</v>
-      </c>
-      <c r="N9" s="3">
-        <v>1</v>
-      </c>
-      <c r="O9" s="3">
-        <v>1</v>
-      </c>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="M9" s="3">
+        <v>2</v>
+      </c>
+      <c r="N9" s="4">
+        <v>1</v>
+      </c>
+      <c r="O9" s="4">
+        <v>1</v>
+      </c>
+      <c r="P9" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>1</v>
+      </c>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
@@ -911,8 +933,10 @@
       <c r="X9" s="3"/>
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -923,46 +947,50 @@
         <v>45</v>
       </c>
       <c r="D10" s="4">
+        <v>45</v>
+      </c>
+      <c r="E10" s="4">
+        <v>45</v>
+      </c>
+      <c r="F10" s="4">
         <v>17</v>
       </c>
-      <c r="E10" s="4">
+      <c r="G10" s="4">
         <v>17</v>
-      </c>
-      <c r="F10" s="4">
-        <v>5</v>
-      </c>
-      <c r="G10" s="4">
-        <v>5</v>
       </c>
       <c r="H10" s="4">
         <v>5</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="4">
         <v>5</v>
       </c>
       <c r="J10" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K10" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L10" s="4">
-        <v>3</v>
-      </c>
-      <c r="M10" s="4">
-        <v>3</v>
-      </c>
-      <c r="N10" s="3">
-        <v>3</v>
-      </c>
-      <c r="O10" s="3">
+        <v>4</v>
+      </c>
+      <c r="M10" s="3">
+        <v>3</v>
+      </c>
+      <c r="N10" s="4">
+        <v>3</v>
+      </c>
+      <c r="O10" s="4">
         <v>3</v>
       </c>
       <c r="P10" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>3</v>
+      </c>
+      <c r="R10" s="3">
+        <v>1</v>
+      </c>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
@@ -971,61 +999,63 @@
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="4">
+        <v>117</v>
+      </c>
+      <c r="C11" s="4">
         <v>67</v>
       </c>
-      <c r="C11" s="4">
-        <v>28</v>
-      </c>
       <c r="D11" s="4">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="E11" s="4">
         <v>28</v>
       </c>
       <c r="F11" s="4">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="G11" s="4">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="H11" s="4">
         <v>9</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="4">
         <v>9</v>
       </c>
       <c r="J11" s="4">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="K11" s="3">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="L11" s="4">
         <v>4</v>
       </c>
-      <c r="M11" s="4">
-        <v>3</v>
-      </c>
-      <c r="N11" s="3">
-        <v>3</v>
-      </c>
-      <c r="O11" s="3">
+      <c r="M11" s="3">
+        <v>4</v>
+      </c>
+      <c r="N11" s="4">
+        <v>4</v>
+      </c>
+      <c r="O11" s="4">
         <v>3</v>
       </c>
       <c r="P11" s="3">
         <v>3</v>
       </c>
       <c r="Q11" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R11" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S11" s="3">
         <v>1</v>
@@ -1045,139 +1075,151 @@
       <c r="X11" s="3">
         <v>1</v>
       </c>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Y11" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="4">
+        <v>83</v>
+      </c>
+      <c r="C12" s="4">
         <v>71</v>
       </c>
-      <c r="C12" s="4">
+      <c r="D12" s="4">
+        <v>71</v>
+      </c>
+      <c r="E12" s="4">
         <v>62</v>
       </c>
-      <c r="D12" s="4">
+      <c r="F12" s="4">
         <v>39</v>
       </c>
-      <c r="E12" s="4">
+      <c r="G12" s="4">
         <v>31</v>
       </c>
-      <c r="F12" s="4">
+      <c r="H12" s="4">
         <v>29</v>
       </c>
-      <c r="G12" s="4">
+      <c r="I12" s="4">
         <v>13</v>
       </c>
-      <c r="H12" s="4">
+      <c r="J12" s="4">
         <v>13</v>
       </c>
-      <c r="I12" s="3">
+      <c r="K12" s="3">
         <v>8</v>
       </c>
-      <c r="J12" s="4">
-        <v>4</v>
-      </c>
-      <c r="K12" s="3">
+      <c r="L12" s="4">
+        <v>4</v>
+      </c>
+      <c r="M12" s="3">
         <v>6</v>
       </c>
-      <c r="L12" s="4">
+      <c r="N12" s="4">
         <v>5</v>
       </c>
-      <c r="M12" s="4">
-        <v>4</v>
-      </c>
-      <c r="N12" s="3">
-        <v>4</v>
-      </c>
-      <c r="O12" s="3">
+      <c r="O12" s="4">
         <v>4</v>
       </c>
       <c r="P12" s="3">
         <v>4</v>
       </c>
       <c r="Q12" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R12" s="3">
-        <v>1</v>
-      </c>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="S12" s="3">
+        <v>3</v>
+      </c>
+      <c r="T12" s="3">
+        <v>1</v>
+      </c>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="4">
+        <v>167</v>
+      </c>
+      <c r="C13" s="4">
         <v>134</v>
       </c>
-      <c r="C13" s="4">
+      <c r="D13" s="4">
+        <v>134</v>
+      </c>
+      <c r="E13" s="4">
         <v>101</v>
       </c>
-      <c r="D13" s="4">
+      <c r="F13" s="4">
         <v>78</v>
       </c>
-      <c r="E13" s="4">
+      <c r="G13" s="4">
         <v>54</v>
       </c>
-      <c r="F13" s="4">
+      <c r="H13" s="4">
         <v>45</v>
       </c>
-      <c r="G13" s="4">
+      <c r="I13" s="4">
         <v>42</v>
       </c>
-      <c r="H13" s="4">
+      <c r="J13" s="4">
         <v>26</v>
       </c>
-      <c r="I13" s="3">
+      <c r="K13" s="3">
         <v>19</v>
       </c>
-      <c r="J13" s="4">
+      <c r="L13" s="4">
         <v>18</v>
       </c>
-      <c r="K13" s="3">
+      <c r="M13" s="3">
         <v>12</v>
       </c>
-      <c r="L13" s="4">
+      <c r="N13" s="4">
         <v>6</v>
       </c>
-      <c r="M13" s="4">
+      <c r="O13" s="4">
         <v>6</v>
       </c>
-      <c r="N13" s="3">
+      <c r="P13" s="3">
         <v>5</v>
       </c>
-      <c r="O13" s="3">
+      <c r="Q13" s="3">
         <v>5</v>
       </c>
-      <c r="P13" s="3">
-        <v>4</v>
-      </c>
-      <c r="Q13" s="3">
-        <v>4</v>
-      </c>
       <c r="R13" s="3">
         <v>4</v>
       </c>
       <c r="S13" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="T13" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U13" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V13" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W13" s="3">
         <v>3</v>
@@ -1185,60 +1227,70 @@
       <c r="X13" s="3">
         <v>3</v>
       </c>
-      <c r="Y13" s="3"/>
-      <c r="Z13" s="3"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Y13" s="3">
+        <v>3</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>3</v>
+      </c>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="4">
+        <v>120</v>
+      </c>
+      <c r="C14" s="4">
+        <v>108</v>
+      </c>
+      <c r="D14" s="4">
         <v>92</v>
       </c>
-      <c r="C14" s="4">
+      <c r="E14" s="4">
         <v>76</v>
       </c>
-      <c r="D14" s="4">
+      <c r="F14" s="4">
         <v>61</v>
       </c>
-      <c r="E14" s="4">
+      <c r="G14" s="4">
         <v>51</v>
       </c>
-      <c r="F14" s="4">
+      <c r="H14" s="4">
         <v>43</v>
       </c>
-      <c r="G14" s="4">
+      <c r="I14" s="4">
         <v>34</v>
       </c>
-      <c r="H14" s="4">
+      <c r="J14" s="4">
         <v>26</v>
       </c>
-      <c r="I14" s="3">
+      <c r="K14" s="3">
         <v>15</v>
       </c>
-      <c r="J14" s="4">
+      <c r="L14" s="4">
         <v>12</v>
       </c>
-      <c r="K14" s="3">
+      <c r="M14" s="3">
         <v>7</v>
       </c>
-      <c r="L14" s="4">
+      <c r="N14" s="4">
         <v>6</v>
       </c>
-      <c r="M14" s="4">
-        <v>2</v>
-      </c>
-      <c r="N14" s="3">
-        <v>1</v>
-      </c>
-      <c r="O14" s="3">
-        <v>1</v>
+      <c r="O14" s="4">
+        <v>2</v>
       </c>
       <c r="P14" s="3">
         <v>1</v>
       </c>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
+      <c r="Q14" s="3">
+        <v>1</v>
+      </c>
+      <c r="R14" s="3">
+        <v>1</v>
+      </c>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
@@ -1247,119 +1299,131 @@
       <c r="X14" s="3"/>
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="11">
+        <v>121</v>
+      </c>
+      <c r="C15" s="11">
         <v>110</v>
       </c>
-      <c r="C15" s="11">
+      <c r="D15" s="11">
+        <v>110</v>
+      </c>
+      <c r="E15" s="11">
         <v>99</v>
       </c>
-      <c r="D15" s="11">
+      <c r="F15" s="11">
         <v>60</v>
       </c>
-      <c r="E15" s="11">
+      <c r="G15" s="11">
         <v>59</v>
       </c>
-      <c r="F15" s="11">
+      <c r="H15" s="11">
         <v>35</v>
       </c>
-      <c r="G15" s="11">
+      <c r="I15" s="11">
         <v>35</v>
       </c>
-      <c r="H15" s="11">
+      <c r="J15" s="11">
         <v>21</v>
       </c>
-      <c r="I15" s="3">
+      <c r="K15" s="3">
         <v>17</v>
       </c>
-      <c r="J15" s="11">
+      <c r="L15" s="11">
         <v>16</v>
       </c>
-      <c r="K15" s="3">
+      <c r="M15" s="3">
         <v>15</v>
       </c>
-      <c r="L15" s="11">
+      <c r="N15" s="11">
         <v>13</v>
       </c>
-      <c r="M15" s="11">
+      <c r="O15" s="11">
         <v>13</v>
       </c>
-      <c r="N15" s="3">
+      <c r="P15" s="3">
         <v>12</v>
       </c>
-      <c r="O15" s="3">
-        <v>3</v>
-      </c>
-      <c r="P15" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3">
-        <v>1</v>
-      </c>
-      <c r="T15" s="3">
-        <v>1</v>
-      </c>
-      <c r="U15" s="3"/>
-      <c r="V15" s="3"/>
+      <c r="Q15" s="3">
+        <v>3</v>
+      </c>
+      <c r="R15" s="3">
+        <v>1</v>
+      </c>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3">
+        <v>1</v>
+      </c>
+      <c r="V15" s="3">
+        <v>1</v>
+      </c>
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="3"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="4">
+        <v>33</v>
+      </c>
+      <c r="C16" s="4">
+        <v>33</v>
+      </c>
+      <c r="D16" s="4">
         <v>24</v>
       </c>
-      <c r="C16" s="4">
+      <c r="E16" s="4">
         <v>21</v>
       </c>
-      <c r="D16" s="4">
+      <c r="F16" s="4">
         <v>12</v>
       </c>
-      <c r="E16" s="4">
+      <c r="G16" s="4">
         <v>9</v>
       </c>
-      <c r="F16" s="4">
-        <v>4</v>
-      </c>
-      <c r="G16" s="4">
-        <v>3</v>
-      </c>
       <c r="H16" s="4">
-        <v>3</v>
-      </c>
-      <c r="I16" s="3">
+        <v>4</v>
+      </c>
+      <c r="I16" s="4">
         <v>3</v>
       </c>
       <c r="J16" s="4">
         <v>3</v>
       </c>
       <c r="K16" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L16" s="4">
-        <v>1</v>
-      </c>
-      <c r="M16" s="4">
-        <v>1</v>
-      </c>
-      <c r="N16" s="3">
-        <v>1</v>
-      </c>
-      <c r="O16" s="3">
-        <v>1</v>
-      </c>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="M16" s="3">
+        <v>2</v>
+      </c>
+      <c r="N16" s="4">
+        <v>1</v>
+      </c>
+      <c r="O16" s="4">
+        <v>1</v>
+      </c>
+      <c r="P16" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>1</v>
+      </c>
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
@@ -1369,148 +1433,162 @@
       <c r="X16" s="3"/>
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="3"/>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="4">
+        <v>362</v>
+      </c>
+      <c r="C17" s="4">
         <v>323</v>
       </c>
-      <c r="C17" s="4">
+      <c r="D17" s="4">
+        <v>323</v>
+      </c>
+      <c r="E17" s="4">
         <v>234</v>
       </c>
-      <c r="D17" s="4">
+      <c r="F17" s="4">
         <v>193</v>
       </c>
-      <c r="E17" s="4">
+      <c r="G17" s="4">
         <v>128</v>
       </c>
-      <c r="F17" s="4">
+      <c r="H17" s="4">
         <v>123</v>
       </c>
-      <c r="G17" s="4">
+      <c r="I17" s="4">
         <v>111</v>
       </c>
-      <c r="H17" s="4">
+      <c r="J17" s="4">
         <v>82</v>
       </c>
-      <c r="I17" s="3">
+      <c r="K17" s="3">
         <v>65</v>
       </c>
-      <c r="J17" s="4">
+      <c r="L17" s="4">
         <v>47</v>
       </c>
-      <c r="K17" s="3">
+      <c r="M17" s="3">
         <v>43</v>
       </c>
-      <c r="L17" s="4">
+      <c r="N17" s="4">
         <v>23</v>
       </c>
-      <c r="M17" s="4">
+      <c r="O17" s="4">
         <v>18</v>
       </c>
-      <c r="N17" s="3">
+      <c r="P17" s="3">
         <v>16</v>
       </c>
-      <c r="O17" s="3">
+      <c r="Q17" s="3">
         <v>16</v>
       </c>
-      <c r="P17" s="3">
+      <c r="R17" s="3">
         <v>14</v>
       </c>
-      <c r="Q17" s="3">
+      <c r="S17" s="3">
         <v>13</v>
       </c>
-      <c r="R17" s="3">
+      <c r="T17" s="3">
         <v>5</v>
       </c>
-      <c r="S17" s="3">
+      <c r="U17" s="3">
         <v>5</v>
       </c>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA17" s="3"/>
+      <c r="AB17" s="3"/>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B18" s="4">
+        <v>191</v>
+      </c>
+      <c r="C18" s="4">
         <v>150</v>
       </c>
-      <c r="C18" s="4">
+      <c r="D18" s="4">
+        <v>150</v>
+      </c>
+      <c r="E18" s="4">
         <v>114</v>
       </c>
-      <c r="D18" s="4">
+      <c r="F18" s="4">
         <v>79</v>
       </c>
-      <c r="E18" s="4">
+      <c r="G18" s="4">
         <v>62</v>
       </c>
-      <c r="F18" s="4">
+      <c r="H18" s="4">
         <v>53</v>
       </c>
-      <c r="G18" s="4">
+      <c r="I18" s="4">
         <v>43</v>
       </c>
-      <c r="H18" s="4">
+      <c r="J18" s="4">
         <v>34</v>
       </c>
-      <c r="I18" s="3">
+      <c r="K18" s="3">
         <v>18</v>
       </c>
-      <c r="J18" s="4">
+      <c r="L18" s="4">
         <v>18</v>
       </c>
-      <c r="K18" s="3">
+      <c r="M18" s="3">
         <v>13</v>
       </c>
-      <c r="L18" s="4">
+      <c r="N18" s="4">
         <v>12</v>
       </c>
-      <c r="M18" s="4">
+      <c r="O18" s="4">
         <v>12</v>
-      </c>
-      <c r="N18" s="3">
-        <v>8</v>
-      </c>
-      <c r="O18" s="3">
-        <v>8</v>
       </c>
       <c r="P18" s="3">
         <v>8</v>
       </c>
       <c r="Q18" s="3">
+        <v>8</v>
+      </c>
+      <c r="R18" s="3">
+        <v>8</v>
+      </c>
+      <c r="S18" s="3">
         <v>6</v>
       </c>
-      <c r="R18" s="3">
+      <c r="T18" s="3">
         <v>6</v>
       </c>
-      <c r="S18" s="3">
-        <v>4</v>
-      </c>
-      <c r="T18" s="3">
-        <v>4</v>
-      </c>
       <c r="U18" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V18" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W18" s="3">
-        <v>1</v>
-      </c>
-      <c r="X18" s="3"/>
-      <c r="Y18" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="X18" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y18" s="3">
+        <v>1</v>
+      </c>
       <c r="Z18" s="3"/>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3"/>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -1524,32 +1602,36 @@
         <v>14</v>
       </c>
       <c r="E19" s="4">
+        <v>14</v>
+      </c>
+      <c r="F19" s="4">
+        <v>14</v>
+      </c>
+      <c r="G19" s="4">
         <v>10</v>
       </c>
-      <c r="F19" s="4">
+      <c r="H19" s="4">
         <v>8</v>
       </c>
-      <c r="G19" s="4">
+      <c r="I19" s="4">
         <v>7</v>
       </c>
-      <c r="H19" s="4">
-        <v>3</v>
-      </c>
-      <c r="I19" s="3">
-        <v>2</v>
-      </c>
       <c r="J19" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L19" s="4">
-        <v>1</v>
-      </c>
-      <c r="M19" s="4"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="M19" s="3">
+        <v>1</v>
+      </c>
+      <c r="N19" s="4">
+        <v>1</v>
+      </c>
+      <c r="O19" s="4"/>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
@@ -1561,8 +1643,10 @@
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA19" s="3"/>
+      <c r="AB19" s="3"/>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>15</v>
       </c>
@@ -1570,49 +1654,49 @@
         <v>97</v>
       </c>
       <c r="C20" s="4">
+        <v>97</v>
+      </c>
+      <c r="D20" s="4">
+        <v>97</v>
+      </c>
+      <c r="E20" s="4">
         <v>60</v>
       </c>
-      <c r="D20" s="4">
+      <c r="F20" s="4">
         <v>59</v>
       </c>
-      <c r="E20" s="4">
+      <c r="G20" s="4">
         <v>39</v>
       </c>
-      <c r="F20" s="4">
+      <c r="H20" s="4">
         <v>29</v>
       </c>
-      <c r="G20" s="4">
+      <c r="I20" s="4">
         <v>16</v>
       </c>
-      <c r="H20" s="4">
+      <c r="J20" s="4">
         <v>16</v>
       </c>
-      <c r="I20" s="3">
+      <c r="K20" s="3">
         <v>14</v>
       </c>
-      <c r="J20" s="4">
-        <v>3</v>
-      </c>
-      <c r="K20" s="3">
-        <v>1</v>
-      </c>
       <c r="L20" s="4">
-        <v>4</v>
-      </c>
-      <c r="M20" s="4">
-        <v>3</v>
-      </c>
-      <c r="N20" s="3">
-        <v>3</v>
-      </c>
-      <c r="O20" s="3">
+        <v>3</v>
+      </c>
+      <c r="M20" s="3">
+        <v>1</v>
+      </c>
+      <c r="N20" s="4">
+        <v>4</v>
+      </c>
+      <c r="O20" s="4">
         <v>3</v>
       </c>
       <c r="P20" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q20" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R20" s="3">
         <v>2</v>
@@ -1633,326 +1717,356 @@
         <v>2</v>
       </c>
       <c r="X20" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y20" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z20" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B21" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C21" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D21" s="4">
         <v>3</v>
       </c>
       <c r="E21" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F21" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G21" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H21" s="4">
-        <v>3</v>
-      </c>
-      <c r="I21" s="3">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="I21" s="4">
+        <v>3</v>
       </c>
       <c r="J21" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K21" s="3">
         <v>2</v>
       </c>
       <c r="L21" s="4">
+        <v>2</v>
+      </c>
+      <c r="M21" s="3">
+        <v>2</v>
+      </c>
+      <c r="N21" s="4">
         <v>5</v>
       </c>
-      <c r="M21" s="4">
+      <c r="O21" s="4">
         <v>5</v>
       </c>
-      <c r="N21" s="3">
+      <c r="P21" s="3">
         <v>5</v>
       </c>
-      <c r="O21" s="3">
+      <c r="Q21" s="3">
         <v>5</v>
       </c>
-      <c r="P21" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q21" s="3">
-        <v>2</v>
-      </c>
       <c r="R21" s="3">
         <v>2</v>
       </c>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
+      <c r="S21" s="3">
+        <v>2</v>
+      </c>
+      <c r="T21" s="3">
+        <v>2</v>
+      </c>
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="3"/>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="4">
+        <v>57</v>
+      </c>
+      <c r="C22" s="4">
+        <v>47</v>
+      </c>
+      <c r="D22" s="4">
         <v>39</v>
       </c>
-      <c r="C22" s="4">
+      <c r="E22" s="4">
         <v>34</v>
       </c>
-      <c r="D22" s="4">
+      <c r="F22" s="4">
         <v>17</v>
       </c>
-      <c r="E22" s="4">
+      <c r="G22" s="4">
         <v>17</v>
       </c>
-      <c r="F22" s="4">
+      <c r="H22" s="4">
         <v>21</v>
       </c>
-      <c r="G22" s="4">
+      <c r="I22" s="4">
         <v>21</v>
       </c>
-      <c r="H22" s="4">
+      <c r="J22" s="4">
         <v>19</v>
       </c>
-      <c r="I22" s="3">
+      <c r="K22" s="3">
         <v>8</v>
       </c>
-      <c r="J22" s="4">
+      <c r="L22" s="4">
         <v>8</v>
       </c>
-      <c r="K22" s="3">
-        <v>4</v>
-      </c>
-      <c r="L22" s="4">
-        <v>3</v>
-      </c>
-      <c r="M22" s="4">
-        <v>3</v>
-      </c>
-      <c r="N22" s="3">
-        <v>3</v>
-      </c>
-      <c r="O22" s="3">
+      <c r="M22" s="3">
+        <v>4</v>
+      </c>
+      <c r="N22" s="4">
+        <v>3</v>
+      </c>
+      <c r="O22" s="4">
         <v>3</v>
       </c>
       <c r="P22" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q22" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R22" s="3">
         <v>1</v>
       </c>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
+      <c r="S22" s="3">
+        <v>1</v>
+      </c>
+      <c r="T22" s="3">
+        <v>1</v>
+      </c>
       <c r="U22" s="3"/>
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3"/>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="11">
+        <v>165</v>
+      </c>
+      <c r="C23" s="11">
+        <v>140</v>
+      </c>
+      <c r="D23" s="11">
         <v>118</v>
       </c>
-      <c r="C23" s="11">
+      <c r="E23" s="11">
         <v>110</v>
       </c>
-      <c r="D23" s="11">
+      <c r="F23" s="11">
         <v>71</v>
       </c>
-      <c r="E23" s="11">
+      <c r="G23" s="11">
         <v>57</v>
       </c>
-      <c r="F23" s="11">
+      <c r="H23" s="11">
         <v>50</v>
       </c>
-      <c r="G23" s="11">
+      <c r="I23" s="11">
         <v>47</v>
       </c>
-      <c r="H23" s="11">
+      <c r="J23" s="11">
         <v>37</v>
       </c>
-      <c r="I23" s="3">
+      <c r="K23" s="3">
         <v>32</v>
       </c>
-      <c r="J23" s="11">
+      <c r="L23" s="11">
         <v>32</v>
       </c>
-      <c r="K23" s="3">
+      <c r="M23" s="3">
         <v>30</v>
       </c>
-      <c r="L23" s="11">
+      <c r="N23" s="11">
         <v>26</v>
       </c>
-      <c r="M23" s="11">
+      <c r="O23" s="11">
         <v>26</v>
       </c>
-      <c r="N23" s="3">
+      <c r="P23" s="3">
         <v>20</v>
       </c>
-      <c r="O23" s="3">
+      <c r="Q23" s="3">
         <v>20</v>
       </c>
-      <c r="P23" s="3">
+      <c r="R23" s="3">
         <v>14</v>
       </c>
-      <c r="Q23" s="3">
+      <c r="S23" s="3">
         <v>10</v>
       </c>
-      <c r="R23" s="3">
+      <c r="T23" s="3">
         <v>10</v>
       </c>
-      <c r="S23" s="3">
+      <c r="U23" s="3">
         <v>8</v>
       </c>
-      <c r="T23" s="3">
+      <c r="V23" s="3">
         <v>8</v>
       </c>
-      <c r="U23" s="3">
-        <v>1</v>
-      </c>
-      <c r="V23" s="3">
-        <v>1</v>
-      </c>
       <c r="W23" s="3">
         <v>1</v>
       </c>
-      <c r="X23" s="3"/>
-      <c r="Y23" s="3"/>
+      <c r="X23" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="3">
+        <v>1</v>
+      </c>
       <c r="Z23" s="3"/>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="3"/>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>43</v>
       </c>
       <c r="B24" s="11">
+        <v>28</v>
+      </c>
+      <c r="C24" s="11">
         <v>20</v>
       </c>
-      <c r="C24" s="11">
+      <c r="D24" s="11">
+        <v>20</v>
+      </c>
+      <c r="E24" s="11">
         <v>19</v>
       </c>
-      <c r="D24" s="11">
+      <c r="F24" s="11">
         <v>13</v>
       </c>
-      <c r="E24" s="11">
+      <c r="G24" s="11">
         <v>9</v>
       </c>
-      <c r="F24" s="11">
-        <v>4</v>
-      </c>
-      <c r="G24" s="11">
-        <v>4</v>
-      </c>
       <c r="H24" s="11">
         <v>4</v>
       </c>
-      <c r="I24" s="3">
-        <v>1</v>
+      <c r="I24" s="11">
+        <v>4</v>
       </c>
       <c r="J24" s="11">
-        <v>1</v>
-      </c>
-      <c r="K24" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="K24" s="3">
+        <v>1</v>
+      </c>
       <c r="L24" s="11">
-        <v>3</v>
-      </c>
-      <c r="M24" s="11">
-        <v>3</v>
-      </c>
-      <c r="N24" s="3">
-        <v>3</v>
-      </c>
-      <c r="O24" s="3">
+        <v>1</v>
+      </c>
+      <c r="M24" s="3"/>
+      <c r="N24" s="11">
+        <v>3</v>
+      </c>
+      <c r="O24" s="11">
         <v>3</v>
       </c>
       <c r="P24" s="3">
         <v>3</v>
       </c>
       <c r="Q24" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R24" s="3">
-        <v>2</v>
-      </c>
-      <c r="S24" s="3"/>
-      <c r="T24" s="3"/>
-      <c r="U24" s="3">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="S24" s="3">
+        <v>2</v>
+      </c>
+      <c r="T24" s="3">
+        <v>2</v>
+      </c>
+      <c r="U24" s="3"/>
       <c r="V24" s="3"/>
-      <c r="W24" s="3"/>
+      <c r="W24" s="3">
+        <v>1</v>
+      </c>
       <c r="X24" s="3"/>
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="3"/>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B25" s="4">
+        <v>222</v>
+      </c>
+      <c r="C25" s="4">
+        <v>222</v>
+      </c>
+      <c r="D25" s="4">
         <v>182</v>
       </c>
-      <c r="C25" s="4">
+      <c r="E25" s="4">
         <v>154</v>
       </c>
-      <c r="D25" s="4">
+      <c r="F25" s="4">
         <v>135</v>
       </c>
-      <c r="E25" s="4">
+      <c r="G25" s="4">
         <v>64</v>
-      </c>
-      <c r="F25" s="4">
-        <v>29</v>
-      </c>
-      <c r="G25" s="4">
-        <v>29</v>
       </c>
       <c r="H25" s="4">
         <v>29</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25" s="4">
+        <v>29</v>
+      </c>
+      <c r="J25" s="4">
+        <v>29</v>
+      </c>
+      <c r="K25" s="3">
         <v>8</v>
       </c>
-      <c r="J25" s="4">
+      <c r="L25" s="4">
         <v>8</v>
       </c>
-      <c r="K25" s="3">
+      <c r="M25" s="3">
         <v>6</v>
       </c>
-      <c r="L25" s="4">
-        <v>2</v>
-      </c>
-      <c r="M25" s="4">
-        <v>2</v>
-      </c>
-      <c r="N25" s="3">
-        <v>1</v>
-      </c>
-      <c r="O25" s="3">
-        <v>1</v>
+      <c r="N25" s="4">
+        <v>2</v>
+      </c>
+      <c r="O25" s="4">
+        <v>2</v>
       </c>
       <c r="P25" s="3">
         <v>1</v>
@@ -1960,8 +2074,12 @@
       <c r="Q25" s="3">
         <v>1</v>
       </c>
-      <c r="R25" s="3"/>
-      <c r="S25" s="3"/>
+      <c r="R25" s="3">
+        <v>1</v>
+      </c>
+      <c r="S25" s="3">
+        <v>1</v>
+      </c>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
       <c r="V25" s="3"/>
@@ -1969,64 +2087,66 @@
       <c r="X25" s="3"/>
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA25" s="3"/>
+      <c r="AB25" s="3"/>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B26" s="11">
+        <v>104</v>
+      </c>
+      <c r="C26" s="11">
         <v>96</v>
       </c>
-      <c r="C26" s="11">
+      <c r="D26" s="11">
+        <v>96</v>
+      </c>
+      <c r="E26" s="11">
         <v>75</v>
       </c>
-      <c r="D26" s="11">
+      <c r="F26" s="11">
         <v>63</v>
       </c>
-      <c r="E26" s="11">
+      <c r="G26" s="11">
         <v>47</v>
       </c>
-      <c r="F26" s="11">
+      <c r="H26" s="11">
         <v>24</v>
       </c>
-      <c r="G26" s="11">
+      <c r="I26" s="11">
         <v>29</v>
       </c>
-      <c r="H26" s="11">
+      <c r="J26" s="11">
         <v>29</v>
       </c>
-      <c r="I26" s="3">
+      <c r="K26" s="3">
         <v>16</v>
       </c>
-      <c r="J26" s="11">
+      <c r="L26" s="11">
         <v>16</v>
       </c>
-      <c r="K26" s="3">
+      <c r="M26" s="3">
         <v>12</v>
       </c>
-      <c r="L26" s="11">
+      <c r="N26" s="11">
         <v>9</v>
       </c>
-      <c r="M26" s="11">
+      <c r="O26" s="11">
         <v>7</v>
       </c>
-      <c r="N26" s="3">
+      <c r="P26" s="3">
         <v>7</v>
       </c>
-      <c r="O26" s="3">
+      <c r="Q26" s="3">
         <v>7</v>
       </c>
-      <c r="P26" s="3">
-        <v>3</v>
-      </c>
-      <c r="Q26" s="3">
-        <v>2</v>
-      </c>
       <c r="R26" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S26" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T26" s="3">
         <v>1</v>
@@ -2040,11 +2160,17 @@
       <c r="W26" s="3">
         <v>1</v>
       </c>
-      <c r="X26" s="3"/>
-      <c r="Y26" s="3"/>
+      <c r="X26" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="3">
+        <v>1</v>
+      </c>
       <c r="Z26" s="3"/>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3"/>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>48</v>
       </c>
@@ -2052,38 +2178,42 @@
         <v>42</v>
       </c>
       <c r="C27" s="11">
+        <v>42</v>
+      </c>
+      <c r="D27" s="11">
+        <v>42</v>
+      </c>
+      <c r="E27" s="11">
         <v>34</v>
       </c>
-      <c r="D27" s="11">
+      <c r="F27" s="11">
         <v>29</v>
       </c>
-      <c r="E27" s="11">
+      <c r="G27" s="11">
         <v>26</v>
-      </c>
-      <c r="F27" s="11">
-        <v>14</v>
-      </c>
-      <c r="G27" s="11">
-        <v>14</v>
       </c>
       <c r="H27" s="11">
         <v>14</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I27" s="11">
+        <v>14</v>
+      </c>
+      <c r="J27" s="11">
+        <v>14</v>
+      </c>
+      <c r="K27" s="3">
         <v>8</v>
       </c>
-      <c r="J27" s="11">
+      <c r="L27" s="11">
         <v>8</v>
       </c>
-      <c r="K27" s="3">
-        <v>3</v>
-      </c>
-      <c r="L27" s="11">
-        <v>2</v>
-      </c>
-      <c r="M27" s="11"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
+      <c r="M27" s="3">
+        <v>3</v>
+      </c>
+      <c r="N27" s="11">
+        <v>2</v>
+      </c>
+      <c r="O27" s="11"/>
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
@@ -2095,8 +2225,10 @@
       <c r="X27" s="3"/>
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA27" s="3"/>
+      <c r="AB27" s="3"/>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>29</v>
       </c>
@@ -2104,46 +2236,50 @@
         <v>52</v>
       </c>
       <c r="C28" s="4">
+        <v>52</v>
+      </c>
+      <c r="D28" s="4">
+        <v>52</v>
+      </c>
+      <c r="E28" s="4">
         <v>43</v>
       </c>
-      <c r="D28" s="4">
+      <c r="F28" s="4">
         <v>34</v>
       </c>
-      <c r="E28" s="4">
+      <c r="G28" s="4">
         <v>28</v>
-      </c>
-      <c r="F28" s="4">
-        <v>20</v>
-      </c>
-      <c r="G28" s="4">
-        <v>20</v>
       </c>
       <c r="H28" s="4">
         <v>20</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I28" s="4">
+        <v>20</v>
+      </c>
+      <c r="J28" s="4">
+        <v>20</v>
+      </c>
+      <c r="K28" s="3">
         <v>7</v>
       </c>
-      <c r="J28" s="4">
-        <v>2</v>
-      </c>
-      <c r="K28" s="3">
-        <v>2</v>
-      </c>
       <c r="L28" s="4">
-        <v>1</v>
-      </c>
-      <c r="M28" s="4">
-        <v>1</v>
-      </c>
-      <c r="N28" s="3">
-        <v>1</v>
-      </c>
-      <c r="O28" s="3">
-        <v>1</v>
-      </c>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="M28" s="3">
+        <v>2</v>
+      </c>
+      <c r="N28" s="4">
+        <v>1</v>
+      </c>
+      <c r="O28" s="4">
+        <v>1</v>
+      </c>
+      <c r="P28" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>1</v>
+      </c>
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
@@ -2153,8 +2289,10 @@
       <c r="X28" s="3"/>
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="3"/>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>32</v>
       </c>
@@ -2162,40 +2300,40 @@
         <v>57</v>
       </c>
       <c r="C29" s="4">
+        <v>57</v>
+      </c>
+      <c r="D29" s="4">
+        <v>57</v>
+      </c>
+      <c r="E29" s="4">
         <v>41</v>
       </c>
-      <c r="D29" s="4">
+      <c r="F29" s="4">
         <v>25</v>
       </c>
-      <c r="E29" s="4">
+      <c r="G29" s="4">
         <v>16</v>
-      </c>
-      <c r="F29" s="4">
-        <v>10</v>
-      </c>
-      <c r="G29" s="4">
-        <v>10</v>
       </c>
       <c r="H29" s="4">
         <v>10</v>
       </c>
-      <c r="I29" s="3">
+      <c r="I29" s="4">
+        <v>10</v>
+      </c>
+      <c r="J29" s="4">
+        <v>10</v>
+      </c>
+      <c r="K29" s="3">
         <v>6</v>
       </c>
-      <c r="J29" s="4">
-        <v>4</v>
-      </c>
-      <c r="K29" s="3"/>
       <c r="L29" s="4">
-        <v>1</v>
-      </c>
-      <c r="M29" s="4">
-        <v>1</v>
-      </c>
-      <c r="N29" s="3">
-        <v>1</v>
-      </c>
-      <c r="O29" s="3">
+        <v>4</v>
+      </c>
+      <c r="M29" s="3"/>
+      <c r="N29" s="4">
+        <v>1</v>
+      </c>
+      <c r="O29" s="4">
         <v>1</v>
       </c>
       <c r="P29" s="3">
@@ -2210,77 +2348,83 @@
       <c r="S29" s="3">
         <v>1</v>
       </c>
-      <c r="T29" s="3"/>
-      <c r="U29" s="3"/>
+      <c r="T29" s="3">
+        <v>1</v>
+      </c>
+      <c r="U29" s="3">
+        <v>1</v>
+      </c>
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
       <c r="X29" s="3"/>
       <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA29" s="3"/>
+      <c r="AB29" s="3"/>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="4">
+        <v>236</v>
+      </c>
+      <c r="C30" s="4">
         <v>175</v>
       </c>
-      <c r="C30" s="4">
+      <c r="D30" s="4">
+        <v>175</v>
+      </c>
+      <c r="E30" s="4">
         <v>126</v>
       </c>
-      <c r="D30" s="4">
+      <c r="F30" s="4">
         <v>112</v>
       </c>
-      <c r="E30" s="4">
+      <c r="G30" s="4">
         <v>87</v>
-      </c>
-      <c r="F30" s="4">
-        <v>38</v>
-      </c>
-      <c r="G30" s="4">
-        <v>38</v>
       </c>
       <c r="H30" s="4">
         <v>38</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I30" s="4">
+        <v>38</v>
+      </c>
+      <c r="J30" s="4">
+        <v>38</v>
+      </c>
+      <c r="K30" s="3">
         <v>24</v>
       </c>
-      <c r="J30" s="4">
+      <c r="L30" s="4">
         <v>18</v>
       </c>
-      <c r="K30" s="3">
+      <c r="M30" s="3">
         <v>11</v>
       </c>
-      <c r="L30" s="4">
+      <c r="N30" s="4">
         <v>11</v>
       </c>
-      <c r="M30" s="4">
+      <c r="O30" s="4">
         <v>8</v>
       </c>
-      <c r="N30" s="3">
+      <c r="P30" s="3">
         <v>7</v>
       </c>
-      <c r="O30" s="3">
+      <c r="Q30" s="3">
         <v>7</v>
       </c>
-      <c r="P30" s="3">
+      <c r="R30" s="3">
         <v>5</v>
       </c>
-      <c r="Q30" s="3">
-        <v>3</v>
-      </c>
-      <c r="R30" s="3">
-        <v>3</v>
-      </c>
       <c r="S30" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T30" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U30" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V30" s="3">
         <v>1</v>
@@ -2288,11 +2432,17 @@
       <c r="W30" s="3">
         <v>1</v>
       </c>
-      <c r="X30" s="3"/>
-      <c r="Y30" s="3"/>
+      <c r="X30" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y30" s="3">
+        <v>1</v>
+      </c>
       <c r="Z30" s="3"/>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="3"/>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>3</v>
       </c>
@@ -2300,13 +2450,13 @@
         <v>36</v>
       </c>
       <c r="C31" s="4">
+        <v>36</v>
+      </c>
+      <c r="D31" s="4">
+        <v>36</v>
+      </c>
+      <c r="E31" s="4">
         <v>33</v>
-      </c>
-      <c r="D31" s="4">
-        <v>31</v>
-      </c>
-      <c r="E31" s="4">
-        <v>31</v>
       </c>
       <c r="F31" s="4">
         <v>31</v>
@@ -2315,48 +2465,54 @@
         <v>31</v>
       </c>
       <c r="H31" s="4">
+        <v>31</v>
+      </c>
+      <c r="I31" s="4">
+        <v>31</v>
+      </c>
+      <c r="J31" s="4">
         <v>30</v>
       </c>
-      <c r="I31" s="3">
+      <c r="K31" s="3">
         <v>28</v>
-      </c>
-      <c r="J31" s="4">
-        <v>24</v>
-      </c>
-      <c r="K31" s="3">
-        <v>24</v>
       </c>
       <c r="L31" s="4">
         <v>24</v>
       </c>
-      <c r="M31" s="4">
+      <c r="M31" s="3">
         <v>24</v>
       </c>
-      <c r="N31" s="3">
+      <c r="N31" s="4">
+        <v>24</v>
+      </c>
+      <c r="O31" s="4">
+        <v>24</v>
+      </c>
+      <c r="P31" s="3">
         <v>23</v>
       </c>
-      <c r="O31" s="3">
+      <c r="Q31" s="3">
         <v>23</v>
       </c>
-      <c r="P31" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q31" s="3">
-        <v>1</v>
-      </c>
       <c r="R31" s="3">
-        <v>1</v>
-      </c>
-      <c r="S31" s="3"/>
-      <c r="T31" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="S31" s="3">
+        <v>1</v>
+      </c>
+      <c r="T31" s="3">
+        <v>1</v>
+      </c>
       <c r="U31" s="3"/>
       <c r="V31" s="3"/>
       <c r="W31" s="3"/>
       <c r="X31" s="3"/>
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA31" s="3"/>
+      <c r="AB31" s="3"/>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>44</v>
       </c>
@@ -2364,16 +2520,16 @@
         <v>80</v>
       </c>
       <c r="C32" s="4">
+        <v>80</v>
+      </c>
+      <c r="D32" s="4">
+        <v>80</v>
+      </c>
+      <c r="E32" s="4">
         <v>73</v>
       </c>
-      <c r="D32" s="4">
+      <c r="F32" s="4">
         <v>71</v>
-      </c>
-      <c r="E32" s="4">
-        <v>27</v>
-      </c>
-      <c r="F32" s="4">
-        <v>27</v>
       </c>
       <c r="G32" s="4">
         <v>27</v>
@@ -2381,102 +2537,112 @@
       <c r="H32" s="4">
         <v>27</v>
       </c>
-      <c r="I32" s="3">
+      <c r="I32" s="4">
+        <v>27</v>
+      </c>
+      <c r="J32" s="4">
+        <v>27</v>
+      </c>
+      <c r="K32" s="3">
         <v>22</v>
       </c>
-      <c r="J32" s="4">
+      <c r="L32" s="4">
         <v>12</v>
       </c>
-      <c r="K32" s="3">
+      <c r="M32" s="3">
         <v>12</v>
       </c>
-      <c r="L32" s="4">
+      <c r="N32" s="4">
         <v>9</v>
       </c>
-      <c r="M32" s="4">
+      <c r="O32" s="4">
         <v>9</v>
       </c>
-      <c r="N32" s="3">
+      <c r="P32" s="3">
         <v>7</v>
       </c>
-      <c r="O32" s="3">
+      <c r="Q32" s="3">
         <v>7</v>
       </c>
-      <c r="P32" s="3">
+      <c r="R32" s="3">
         <v>5</v>
       </c>
-      <c r="Q32" s="3">
-        <v>4</v>
-      </c>
-      <c r="R32" s="3">
-        <v>4</v>
-      </c>
       <c r="S32" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="T32" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U32" s="3">
         <v>3</v>
       </c>
-      <c r="V32" s="3"/>
-      <c r="W32" s="3"/>
+      <c r="V32" s="3">
+        <v>3</v>
+      </c>
+      <c r="W32" s="3">
+        <v>3</v>
+      </c>
       <c r="X32" s="3"/>
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA32" s="3"/>
+      <c r="AB32" s="3"/>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B33" s="4">
+        <v>30</v>
+      </c>
+      <c r="C33" s="4">
         <v>26</v>
       </c>
-      <c r="C33" s="4">
+      <c r="D33" s="4">
+        <v>26</v>
+      </c>
+      <c r="E33" s="4">
         <v>20</v>
       </c>
-      <c r="D33" s="4">
+      <c r="F33" s="4">
         <v>17</v>
       </c>
-      <c r="E33" s="4">
+      <c r="G33" s="4">
         <v>14</v>
       </c>
-      <c r="F33" s="4">
+      <c r="H33" s="4">
         <v>7</v>
       </c>
-      <c r="G33" s="4">
+      <c r="I33" s="4">
         <v>10</v>
       </c>
-      <c r="H33" s="4">
+      <c r="J33" s="4">
         <v>6</v>
       </c>
-      <c r="I33" s="3">
-        <v>4</v>
-      </c>
-      <c r="J33" s="4">
-        <v>2</v>
-      </c>
       <c r="K33" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L33" s="4">
-        <v>1</v>
-      </c>
-      <c r="M33" s="4">
-        <v>1</v>
-      </c>
-      <c r="N33" s="3">
-        <v>1</v>
-      </c>
-      <c r="O33" s="3">
+        <v>2</v>
+      </c>
+      <c r="M33" s="3">
+        <v>2</v>
+      </c>
+      <c r="N33" s="4">
+        <v>1</v>
+      </c>
+      <c r="O33" s="4">
         <v>1</v>
       </c>
       <c r="P33" s="3">
         <v>1</v>
       </c>
-      <c r="Q33" s="3"/>
-      <c r="R33" s="3"/>
+      <c r="Q33" s="3">
+        <v>1</v>
+      </c>
+      <c r="R33" s="3">
+        <v>1</v>
+      </c>
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
       <c r="U33" s="3"/>
@@ -2485,58 +2651,64 @@
       <c r="X33" s="3"/>
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
-    </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA33" s="3"/>
+      <c r="AB33" s="3"/>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B34" s="4">
+        <v>82</v>
+      </c>
+      <c r="C34" s="4">
         <v>71</v>
       </c>
-      <c r="C34" s="4">
+      <c r="D34" s="4">
+        <v>71</v>
+      </c>
+      <c r="E34" s="4">
         <v>55</v>
       </c>
-      <c r="D34" s="4">
+      <c r="F34" s="4">
         <v>45</v>
       </c>
-      <c r="E34" s="4">
+      <c r="G34" s="4">
         <v>38</v>
       </c>
-      <c r="F34" s="4">
+      <c r="H34" s="4">
         <v>28</v>
       </c>
-      <c r="G34" s="4">
+      <c r="I34" s="4">
         <v>25</v>
       </c>
-      <c r="H34" s="4">
+      <c r="J34" s="4">
         <v>22</v>
       </c>
-      <c r="I34" s="3">
+      <c r="K34" s="3">
         <v>16</v>
       </c>
-      <c r="J34" s="4">
+      <c r="L34" s="4">
         <v>13</v>
       </c>
-      <c r="K34" s="3">
+      <c r="M34" s="3">
         <v>13</v>
       </c>
-      <c r="L34" s="4">
+      <c r="N34" s="4">
         <v>12</v>
       </c>
-      <c r="M34" s="4">
+      <c r="O34" s="4">
         <v>12</v>
       </c>
-      <c r="N34" s="3">
+      <c r="P34" s="3">
         <v>7</v>
       </c>
-      <c r="O34" s="3">
+      <c r="Q34" s="3">
         <v>6</v>
       </c>
-      <c r="P34" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q34" s="3"/>
-      <c r="R34" s="3"/>
+      <c r="R34" s="3">
+        <v>2</v>
+      </c>
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
       <c r="U34" s="3"/>
@@ -2545,52 +2717,54 @@
       <c r="X34" s="3"/>
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
-    </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA34" s="3"/>
+      <c r="AB34" s="3"/>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B35" s="4">
+        <v>113</v>
+      </c>
+      <c r="C35" s="4">
         <v>91</v>
       </c>
-      <c r="C35" s="4">
+      <c r="D35" s="4">
+        <v>91</v>
+      </c>
+      <c r="E35" s="4">
         <v>85</v>
       </c>
-      <c r="D35" s="4">
+      <c r="F35" s="4">
         <v>46</v>
       </c>
-      <c r="E35" s="4">
+      <c r="G35" s="4">
         <v>41</v>
       </c>
-      <c r="F35" s="4">
+      <c r="H35" s="4">
         <v>31</v>
       </c>
-      <c r="G35" s="4">
+      <c r="I35" s="4">
         <v>31</v>
       </c>
-      <c r="H35" s="4">
+      <c r="J35" s="4">
         <v>20</v>
       </c>
-      <c r="I35" s="3">
+      <c r="K35" s="3">
         <v>13</v>
       </c>
-      <c r="J35" s="4">
+      <c r="L35" s="4">
         <v>7</v>
       </c>
-      <c r="K35" s="3">
+      <c r="M35" s="3">
         <v>5</v>
       </c>
-      <c r="L35" s="4">
-        <v>4</v>
-      </c>
-      <c r="M35" s="4">
-        <v>4</v>
-      </c>
-      <c r="N35" s="3">
-        <v>3</v>
-      </c>
-      <c r="O35" s="3">
-        <v>3</v>
+      <c r="N35" s="4">
+        <v>4</v>
+      </c>
+      <c r="O35" s="4">
+        <v>4</v>
       </c>
       <c r="P35" s="3">
         <v>3</v>
@@ -2602,54 +2776,64 @@
         <v>3</v>
       </c>
       <c r="S35" s="3">
-        <v>1</v>
-      </c>
-      <c r="T35" s="3"/>
-      <c r="U35" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="T35" s="3">
+        <v>3</v>
+      </c>
+      <c r="U35" s="3">
+        <v>1</v>
+      </c>
       <c r="V35" s="3"/>
       <c r="W35" s="3"/>
       <c r="X35" s="3"/>
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
-    </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA35" s="3"/>
+      <c r="AB35" s="3"/>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B36" s="4">
+        <v>16</v>
+      </c>
+      <c r="C36" s="4">
+        <v>16</v>
+      </c>
+      <c r="D36" s="4">
         <v>14</v>
       </c>
-      <c r="C36" s="4">
+      <c r="E36" s="4">
         <v>11</v>
       </c>
-      <c r="D36" s="4">
+      <c r="F36" s="4">
         <v>7</v>
       </c>
-      <c r="E36" s="4">
+      <c r="G36" s="4">
         <v>6</v>
       </c>
-      <c r="F36" s="4">
+      <c r="H36" s="4">
         <v>5</v>
       </c>
-      <c r="G36" s="4">
-        <v>4</v>
-      </c>
-      <c r="H36" s="4">
-        <v>4</v>
-      </c>
-      <c r="I36" s="3">
+      <c r="I36" s="4">
         <v>4</v>
       </c>
       <c r="J36" s="4">
         <v>4</v>
       </c>
       <c r="K36" s="3">
-        <v>3</v>
-      </c>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="L36" s="4">
+        <v>4</v>
+      </c>
+      <c r="M36" s="3">
+        <v>3</v>
+      </c>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
       <c r="R36" s="3"/>
@@ -2661,55 +2845,61 @@
       <c r="X36" s="3"/>
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA36" s="3"/>
+      <c r="AB36" s="3"/>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B37" s="4">
+        <v>100</v>
+      </c>
+      <c r="C37" s="4">
         <v>81</v>
       </c>
-      <c r="C37" s="4">
+      <c r="D37" s="4">
+        <v>81</v>
+      </c>
+      <c r="E37" s="4">
         <v>64</v>
       </c>
-      <c r="D37" s="4">
+      <c r="F37" s="4">
         <v>53</v>
       </c>
-      <c r="E37" s="4">
+      <c r="G37" s="4">
         <v>37</v>
       </c>
-      <c r="F37" s="4">
+      <c r="H37" s="4">
         <v>34</v>
       </c>
-      <c r="G37" s="4">
+      <c r="I37" s="4">
         <v>26</v>
       </c>
-      <c r="H37" s="4">
+      <c r="J37" s="4">
         <v>19</v>
       </c>
-      <c r="I37" s="3">
+      <c r="K37" s="3">
         <v>12</v>
       </c>
-      <c r="J37" s="4">
+      <c r="L37" s="4">
         <v>11</v>
       </c>
-      <c r="K37" s="3">
-        <v>3</v>
-      </c>
-      <c r="L37" s="4">
-        <v>4</v>
-      </c>
-      <c r="M37" s="4">
-        <v>3</v>
-      </c>
-      <c r="N37" s="3">
-        <v>3</v>
-      </c>
-      <c r="O37" s="3">
-        <v>2</v>
-      </c>
-      <c r="P37" s="3"/>
-      <c r="Q37" s="3"/>
+      <c r="M37" s="3">
+        <v>3</v>
+      </c>
+      <c r="N37" s="4">
+        <v>4</v>
+      </c>
+      <c r="O37" s="4">
+        <v>3</v>
+      </c>
+      <c r="P37" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q37" s="3">
+        <v>2</v>
+      </c>
       <c r="R37" s="3"/>
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
@@ -2719,8 +2909,10 @@
       <c r="X37" s="3"/>
       <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA37" s="3"/>
+      <c r="AB37" s="3"/>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>31</v>
       </c>
@@ -2728,52 +2920,56 @@
         <v>110</v>
       </c>
       <c r="C38" s="4">
+        <v>110</v>
+      </c>
+      <c r="D38" s="4">
+        <v>110</v>
+      </c>
+      <c r="E38" s="4">
         <v>88</v>
       </c>
-      <c r="D38" s="4">
+      <c r="F38" s="4">
         <v>55</v>
       </c>
-      <c r="E38" s="4">
+      <c r="G38" s="4">
         <v>13</v>
       </c>
-      <c r="F38" s="4">
+      <c r="H38" s="4">
         <v>12</v>
       </c>
-      <c r="G38" s="4">
+      <c r="I38" s="4">
         <v>8</v>
       </c>
-      <c r="H38" s="4">
+      <c r="J38" s="4">
         <v>8</v>
       </c>
-      <c r="I38" s="3">
+      <c r="K38" s="3">
         <v>8</v>
       </c>
-      <c r="J38" s="4">
+      <c r="L38" s="4">
         <v>5</v>
       </c>
-      <c r="K38" s="3">
+      <c r="M38" s="3">
         <v>5</v>
       </c>
-      <c r="L38" s="4">
+      <c r="N38" s="4">
         <v>6</v>
       </c>
-      <c r="M38" s="4">
-        <v>3</v>
-      </c>
-      <c r="N38" s="3">
-        <v>3</v>
-      </c>
-      <c r="O38" s="3">
-        <v>2</v>
+      <c r="O38" s="4">
+        <v>3</v>
       </c>
       <c r="P38" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q38" s="3">
-        <v>1</v>
-      </c>
-      <c r="R38" s="3"/>
-      <c r="S38" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="R38" s="3">
+        <v>2</v>
+      </c>
+      <c r="S38" s="3">
+        <v>1</v>
+      </c>
       <c r="T38" s="3"/>
       <c r="U38" s="3"/>
       <c r="V38" s="3"/>
@@ -2781,8 +2977,10 @@
       <c r="X38" s="3"/>
       <c r="Y38" s="3"/>
       <c r="Z38" s="3"/>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA38" s="3"/>
+      <c r="AB38" s="3"/>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>8</v>
       </c>
@@ -2790,104 +2988,114 @@
         <v>117</v>
       </c>
       <c r="C39" s="4">
+        <v>117</v>
+      </c>
+      <c r="D39" s="4">
+        <v>117</v>
+      </c>
+      <c r="E39" s="4">
         <v>79</v>
       </c>
-      <c r="D39" s="4">
+      <c r="F39" s="4">
         <v>49</v>
       </c>
-      <c r="E39" s="4">
+      <c r="G39" s="4">
         <v>49</v>
-      </c>
-      <c r="F39" s="4">
-        <v>23</v>
-      </c>
-      <c r="G39" s="4">
-        <v>23</v>
       </c>
       <c r="H39" s="4">
         <v>23</v>
       </c>
-      <c r="I39" s="3">
+      <c r="I39" s="4">
         <v>23</v>
       </c>
       <c r="J39" s="4">
+        <v>23</v>
+      </c>
+      <c r="K39" s="3">
+        <v>23</v>
+      </c>
+      <c r="L39" s="4">
         <v>10</v>
       </c>
-      <c r="K39" s="3">
+      <c r="M39" s="3">
         <v>5</v>
       </c>
-      <c r="L39" s="4">
+      <c r="N39" s="4">
         <v>6</v>
       </c>
-      <c r="M39" s="4">
+      <c r="O39" s="4">
         <v>5</v>
       </c>
-      <c r="N39" s="3">
+      <c r="P39" s="3">
         <v>5</v>
       </c>
-      <c r="O39" s="3">
-        <v>4</v>
-      </c>
-      <c r="P39" s="3">
-        <v>4</v>
-      </c>
       <c r="Q39" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R39" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S39" s="3">
-        <v>1</v>
-      </c>
-      <c r="T39" s="3"/>
-      <c r="U39" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="T39" s="3">
+        <v>2</v>
+      </c>
+      <c r="U39" s="3">
+        <v>1</v>
+      </c>
       <c r="V39" s="3"/>
       <c r="W39" s="3"/>
       <c r="X39" s="3"/>
       <c r="Y39" s="3"/>
       <c r="Z39" s="3"/>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA39" s="3"/>
+      <c r="AB39" s="3"/>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B40" s="4">
+        <v>95</v>
+      </c>
+      <c r="C40" s="4">
+        <v>95</v>
+      </c>
+      <c r="D40" s="4">
         <v>94</v>
       </c>
-      <c r="C40" s="4">
+      <c r="E40" s="4">
         <v>43</v>
       </c>
-      <c r="D40" s="4">
+      <c r="F40" s="4">
         <v>33</v>
       </c>
-      <c r="E40" s="4">
+      <c r="G40" s="4">
         <v>31</v>
       </c>
-      <c r="F40" s="4">
+      <c r="H40" s="4">
         <v>31</v>
       </c>
-      <c r="G40" s="4">
+      <c r="I40" s="4">
         <v>19</v>
       </c>
-      <c r="H40" s="4">
+      <c r="J40" s="4">
         <v>19</v>
       </c>
-      <c r="I40" s="3">
+      <c r="K40" s="3">
         <v>11</v>
       </c>
-      <c r="J40" s="4">
+      <c r="L40" s="4">
         <v>7</v>
       </c>
-      <c r="K40" s="3">
+      <c r="M40" s="3">
         <v>5</v>
       </c>
-      <c r="L40" s="4">
-        <v>1</v>
-      </c>
-      <c r="M40" s="4"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
+      <c r="N40" s="4">
+        <v>1</v>
+      </c>
+      <c r="O40" s="4"/>
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
       <c r="R40" s="3"/>
@@ -2899,67 +3107,69 @@
       <c r="X40" s="3"/>
       <c r="Y40" s="3"/>
       <c r="Z40" s="3"/>
-    </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA40" s="3"/>
+      <c r="AB40" s="3"/>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="4">
+        <v>240</v>
+      </c>
+      <c r="C41" s="4">
+        <v>240</v>
+      </c>
+      <c r="D41" s="4">
         <v>215</v>
       </c>
-      <c r="C41" s="4">
+      <c r="E41" s="4">
         <v>144</v>
       </c>
-      <c r="D41" s="4">
+      <c r="F41" s="4">
         <v>127</v>
       </c>
-      <c r="E41" s="4">
+      <c r="G41" s="4">
         <v>76</v>
-      </c>
-      <c r="F41" s="4">
-        <v>38</v>
-      </c>
-      <c r="G41" s="4">
-        <v>38</v>
       </c>
       <c r="H41" s="4">
         <v>38</v>
       </c>
-      <c r="I41" s="3">
+      <c r="I41" s="4">
+        <v>38</v>
+      </c>
+      <c r="J41" s="4">
+        <v>38</v>
+      </c>
+      <c r="K41" s="3">
         <v>28</v>
       </c>
-      <c r="J41" s="4">
+      <c r="L41" s="4">
         <v>28</v>
       </c>
-      <c r="K41" s="3">
+      <c r="M41" s="3">
         <v>18</v>
       </c>
-      <c r="L41" s="4">
+      <c r="N41" s="4">
         <v>14</v>
       </c>
-      <c r="M41" s="4">
+      <c r="O41" s="4">
         <v>13</v>
       </c>
-      <c r="N41" s="3">
+      <c r="P41" s="3">
         <v>10</v>
       </c>
-      <c r="O41" s="3">
+      <c r="Q41" s="3">
         <v>7</v>
       </c>
-      <c r="P41" s="3">
-        <v>4</v>
-      </c>
-      <c r="Q41" s="3">
-        <v>3</v>
-      </c>
       <c r="R41" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S41" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T41" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U41" s="3">
         <v>1</v>
@@ -2970,54 +3180,60 @@
       <c r="W41" s="3">
         <v>1</v>
       </c>
-      <c r="X41" s="3"/>
-      <c r="Y41" s="3"/>
+      <c r="X41" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y41" s="3">
+        <v>1</v>
+      </c>
       <c r="Z41" s="3"/>
-    </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA41" s="3"/>
+      <c r="AB41" s="3"/>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B42" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C42" s="4">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D42" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E42" s="4">
+        <v>2</v>
+      </c>
+      <c r="F42" s="4">
+        <v>3</v>
+      </c>
+      <c r="G42" s="4">
         <v>5</v>
       </c>
-      <c r="F42" s="4">
-        <v>4</v>
-      </c>
-      <c r="G42" s="4">
-        <v>3</v>
-      </c>
       <c r="H42" s="4">
-        <v>3</v>
-      </c>
-      <c r="I42" s="3">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="I42" s="4">
+        <v>3</v>
       </c>
       <c r="J42" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K42" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L42" s="4">
         <v>1</v>
       </c>
-      <c r="M42" s="4">
-        <v>1</v>
-      </c>
-      <c r="N42" s="3">
-        <v>1</v>
-      </c>
-      <c r="O42" s="3">
+      <c r="M42" s="3">
+        <v>1</v>
+      </c>
+      <c r="N42" s="4">
+        <v>1</v>
+      </c>
+      <c r="O42" s="4">
         <v>1</v>
       </c>
       <c r="P42" s="3">
@@ -3050,48 +3266,58 @@
       <c r="Y42" s="3">
         <v>1</v>
       </c>
-      <c r="Z42" s="3"/>
-    </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Z42" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA42" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB42" s="3"/>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B43" s="4">
+        <v>111</v>
+      </c>
+      <c r="C43" s="4">
         <v>98</v>
       </c>
-      <c r="C43" s="4">
+      <c r="D43" s="4">
+        <v>98</v>
+      </c>
+      <c r="E43" s="4">
         <v>61</v>
       </c>
-      <c r="D43" s="4">
+      <c r="F43" s="4">
         <v>47</v>
       </c>
-      <c r="E43" s="4">
+      <c r="G43" s="4">
         <v>34</v>
-      </c>
-      <c r="F43" s="4">
-        <v>21</v>
-      </c>
-      <c r="G43" s="4">
-        <v>21</v>
       </c>
       <c r="H43" s="4">
         <v>21</v>
       </c>
-      <c r="I43" s="3">
+      <c r="I43" s="4">
+        <v>21</v>
+      </c>
+      <c r="J43" s="4">
+        <v>21</v>
+      </c>
+      <c r="K43" s="3">
         <v>17</v>
       </c>
-      <c r="J43" s="4">
+      <c r="L43" s="4">
         <v>15</v>
       </c>
-      <c r="K43" s="3"/>
-      <c r="L43" s="4">
-        <v>1</v>
-      </c>
-      <c r="M43" s="4">
-        <v>1</v>
-      </c>
-      <c r="N43" s="3"/>
-      <c r="O43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="4">
+        <v>1</v>
+      </c>
+      <c r="O43" s="4">
+        <v>1</v>
+      </c>
       <c r="P43" s="3"/>
       <c r="Q43" s="3"/>
       <c r="R43" s="3"/>
@@ -3103,55 +3329,61 @@
       <c r="X43" s="3"/>
       <c r="Y43" s="3"/>
       <c r="Z43" s="3"/>
-    </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA43" s="3"/>
+      <c r="AB43" s="3"/>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B44" s="4">
+        <v>69</v>
+      </c>
+      <c r="C44" s="4">
+        <v>48</v>
+      </c>
+      <c r="D44" s="4">
         <v>39</v>
       </c>
-      <c r="C44" s="4">
+      <c r="E44" s="4">
         <v>28</v>
       </c>
-      <c r="D44" s="4">
+      <c r="F44" s="4">
         <v>27</v>
       </c>
-      <c r="E44" s="4">
+      <c r="G44" s="4">
         <v>16</v>
-      </c>
-      <c r="F44" s="4">
-        <v>6</v>
-      </c>
-      <c r="G44" s="4">
-        <v>6</v>
       </c>
       <c r="H44" s="4">
         <v>6</v>
       </c>
-      <c r="I44" s="3">
-        <v>3</v>
+      <c r="I44" s="4">
+        <v>6</v>
       </c>
       <c r="J44" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K44" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L44" s="4">
-        <v>1</v>
-      </c>
-      <c r="M44" s="4">
-        <v>1</v>
-      </c>
-      <c r="N44" s="3">
-        <v>1</v>
-      </c>
-      <c r="O44" s="3">
-        <v>1</v>
-      </c>
-      <c r="P44" s="3"/>
-      <c r="Q44" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="M44" s="3">
+        <v>2</v>
+      </c>
+      <c r="N44" s="4">
+        <v>1</v>
+      </c>
+      <c r="O44" s="4">
+        <v>1</v>
+      </c>
+      <c r="P44" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q44" s="3">
+        <v>1</v>
+      </c>
       <c r="R44" s="3"/>
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
@@ -3161,51 +3393,53 @@
       <c r="X44" s="3"/>
       <c r="Y44" s="3"/>
       <c r="Z44" s="3"/>
-    </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA44" s="3"/>
+      <c r="AB44" s="3"/>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B45" s="4">
+        <v>83</v>
+      </c>
+      <c r="C45" s="4">
+        <v>82</v>
+      </c>
+      <c r="D45" s="4">
         <v>67</v>
       </c>
-      <c r="C45" s="4">
+      <c r="E45" s="4">
         <v>41</v>
       </c>
-      <c r="D45" s="4">
+      <c r="F45" s="4">
         <v>28</v>
       </c>
-      <c r="E45" s="4">
+      <c r="G45" s="4">
         <v>22</v>
       </c>
-      <c r="F45" s="4">
+      <c r="H45" s="4">
         <v>16</v>
       </c>
-      <c r="G45" s="4">
+      <c r="I45" s="4">
         <v>12</v>
       </c>
-      <c r="H45" s="4">
+      <c r="J45" s="4">
         <v>12</v>
       </c>
-      <c r="I45" s="3">
+      <c r="K45" s="3">
         <v>6</v>
       </c>
-      <c r="J45" s="4">
-        <v>4</v>
-      </c>
-      <c r="K45" s="3">
-        <v>3</v>
-      </c>
       <c r="L45" s="4">
-        <v>3</v>
-      </c>
-      <c r="M45" s="4">
-        <v>1</v>
-      </c>
-      <c r="N45" s="3">
-        <v>1</v>
-      </c>
-      <c r="O45" s="3">
+        <v>4</v>
+      </c>
+      <c r="M45" s="3">
+        <v>3</v>
+      </c>
+      <c r="N45" s="4">
+        <v>3</v>
+      </c>
+      <c r="O45" s="4">
         <v>1</v>
       </c>
       <c r="P45" s="3">
@@ -3217,124 +3451,136 @@
       <c r="R45" s="3">
         <v>1</v>
       </c>
-      <c r="S45" s="3"/>
-      <c r="T45" s="3"/>
+      <c r="S45" s="3">
+        <v>1</v>
+      </c>
+      <c r="T45" s="3">
+        <v>1</v>
+      </c>
       <c r="U45" s="3"/>
       <c r="V45" s="3"/>
       <c r="W45" s="3"/>
       <c r="X45" s="3"/>
       <c r="Y45" s="3"/>
       <c r="Z45" s="3"/>
-    </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA45" s="3"/>
+      <c r="AB45" s="3"/>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B46" s="4">
+        <v>350</v>
+      </c>
+      <c r="C46" s="4">
         <v>308</v>
       </c>
-      <c r="C46" s="4">
-        <v>196</v>
-      </c>
       <c r="D46" s="4">
-        <v>196</v>
+        <v>308</v>
       </c>
       <c r="E46" s="4">
         <v>196</v>
       </c>
       <c r="F46" s="4">
-        <v>60</v>
+        <v>196</v>
       </c>
       <c r="G46" s="4">
-        <v>60</v>
+        <v>196</v>
       </c>
       <c r="H46" s="4">
         <v>60</v>
       </c>
-      <c r="I46" s="3">
+      <c r="I46" s="4">
+        <v>60</v>
+      </c>
+      <c r="J46" s="4">
+        <v>60</v>
+      </c>
+      <c r="K46" s="3">
         <v>40</v>
       </c>
-      <c r="J46" s="4">
+      <c r="L46" s="4">
         <v>35</v>
       </c>
-      <c r="K46" s="3">
+      <c r="M46" s="3">
         <v>24</v>
       </c>
-      <c r="L46" s="4">
+      <c r="N46" s="4">
         <v>19</v>
       </c>
-      <c r="M46" s="4">
+      <c r="O46" s="4">
         <v>10</v>
       </c>
-      <c r="N46" s="3">
+      <c r="P46" s="3">
         <v>9</v>
       </c>
-      <c r="O46" s="3">
+      <c r="Q46" s="3">
         <v>8</v>
       </c>
-      <c r="P46" s="3">
-        <v>4</v>
-      </c>
-      <c r="Q46" s="3">
-        <v>3</v>
-      </c>
       <c r="R46" s="3">
-        <v>2</v>
-      </c>
-      <c r="S46" s="3"/>
-      <c r="T46" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="S46" s="3">
+        <v>3</v>
+      </c>
+      <c r="T46" s="3">
+        <v>2</v>
+      </c>
       <c r="U46" s="3"/>
       <c r="V46" s="3"/>
       <c r="W46" s="3"/>
       <c r="X46" s="3"/>
       <c r="Y46" s="3"/>
       <c r="Z46" s="3"/>
-    </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA46" s="3"/>
+      <c r="AB46" s="3"/>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B47" s="4">
+        <v>133</v>
+      </c>
+      <c r="C47" s="4">
         <v>112</v>
       </c>
-      <c r="C47" s="4">
+      <c r="D47" s="4">
+        <v>112</v>
+      </c>
+      <c r="E47" s="4">
         <v>93</v>
       </c>
-      <c r="D47" s="4">
+      <c r="F47" s="4">
         <v>85</v>
       </c>
-      <c r="E47" s="4">
+      <c r="G47" s="4">
         <v>67</v>
       </c>
-      <c r="F47" s="4">
+      <c r="H47" s="4">
         <v>61</v>
       </c>
-      <c r="G47" s="4">
+      <c r="I47" s="4">
         <v>41</v>
       </c>
-      <c r="H47" s="4">
+      <c r="J47" s="4">
         <v>23</v>
       </c>
-      <c r="I47" s="3">
+      <c r="K47" s="3">
         <v>9</v>
       </c>
-      <c r="J47" s="4">
+      <c r="L47" s="4">
         <v>9</v>
       </c>
-      <c r="K47" s="3">
-        <v>3</v>
-      </c>
-      <c r="L47" s="4">
+      <c r="M47" s="3">
+        <v>3</v>
+      </c>
+      <c r="N47" s="4">
         <v>5</v>
       </c>
-      <c r="M47" s="4">
-        <v>3</v>
-      </c>
-      <c r="N47" s="3">
-        <v>2</v>
-      </c>
-      <c r="O47" s="3">
-        <v>2</v>
+      <c r="O47" s="4">
+        <v>3</v>
       </c>
       <c r="P47" s="3">
         <v>2</v>
@@ -3366,40 +3612,50 @@
       <c r="Y47" s="3">
         <v>2</v>
       </c>
-      <c r="Z47" s="3"/>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Z47" s="3">
+        <v>2</v>
+      </c>
+      <c r="AA47" s="3">
+        <v>2</v>
+      </c>
+      <c r="AB47" s="3"/>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B48" s="4">
+        <v>15</v>
+      </c>
+      <c r="C48" s="4">
         <v>13</v>
       </c>
-      <c r="C48" s="4">
+      <c r="D48" s="4">
+        <v>13</v>
+      </c>
+      <c r="E48" s="4">
         <v>10</v>
       </c>
-      <c r="D48" s="4">
+      <c r="F48" s="4">
         <v>7</v>
-      </c>
-      <c r="E48" s="4">
-        <v>5</v>
-      </c>
-      <c r="F48" s="4">
-        <v>5</v>
       </c>
       <c r="G48" s="4">
         <v>5</v>
       </c>
       <c r="H48" s="4">
-        <v>3</v>
-      </c>
-      <c r="I48" s="3"/>
-      <c r="J48" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="I48" s="4">
+        <v>5</v>
+      </c>
+      <c r="J48" s="4">
+        <v>3</v>
+      </c>
       <c r="K48" s="3"/>
       <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="3"/>
-      <c r="O48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
       <c r="P48" s="3"/>
       <c r="Q48" s="3"/>
       <c r="R48" s="3"/>
@@ -3411,53 +3667,55 @@
       <c r="X48" s="3"/>
       <c r="Y48" s="3"/>
       <c r="Z48" s="3"/>
-    </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA48" s="3"/>
+      <c r="AB48" s="3"/>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B49" s="4">
+        <v>40</v>
+      </c>
+      <c r="C49" s="4">
         <v>35</v>
       </c>
-      <c r="C49" s="4">
+      <c r="D49" s="4">
+        <v>35</v>
+      </c>
+      <c r="E49" s="4">
         <v>21</v>
       </c>
-      <c r="D49" s="4">
+      <c r="F49" s="4">
         <v>19</v>
       </c>
-      <c r="E49" s="4">
+      <c r="G49" s="4">
         <v>19</v>
       </c>
-      <c r="F49" s="4">
+      <c r="H49" s="4">
         <v>13</v>
       </c>
-      <c r="G49" s="4">
+      <c r="I49" s="4">
         <v>12</v>
       </c>
-      <c r="H49" s="4">
+      <c r="J49" s="4">
         <v>7</v>
-      </c>
-      <c r="I49" s="3">
-        <v>5</v>
-      </c>
-      <c r="J49" s="4">
-        <v>5</v>
       </c>
       <c r="K49" s="3">
         <v>5</v>
       </c>
       <c r="L49" s="4">
+        <v>5</v>
+      </c>
+      <c r="M49" s="3">
+        <v>5</v>
+      </c>
+      <c r="N49" s="4">
         <v>6</v>
       </c>
-      <c r="M49" s="4">
+      <c r="O49" s="4">
         <v>5</v>
       </c>
-      <c r="N49" s="3">
-        <v>4</v>
-      </c>
-      <c r="O49" s="3">
-        <v>4</v>
-      </c>
       <c r="P49" s="3">
         <v>4</v>
       </c>
@@ -3468,52 +3726,62 @@
         <v>4</v>
       </c>
       <c r="S49" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="T49" s="3">
-        <v>1</v>
-      </c>
-      <c r="U49" s="3"/>
-      <c r="V49" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="U49" s="3">
+        <v>1</v>
+      </c>
+      <c r="V49" s="3">
+        <v>1</v>
+      </c>
       <c r="W49" s="3"/>
       <c r="X49" s="3"/>
       <c r="Y49" s="3"/>
       <c r="Z49" s="3"/>
-    </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA49" s="3"/>
+      <c r="AB49" s="3"/>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B50" s="4">
+        <v>15</v>
+      </c>
+      <c r="C50" s="4">
         <v>13</v>
       </c>
-      <c r="C50" s="4">
+      <c r="D50" s="4">
+        <v>13</v>
+      </c>
+      <c r="E50" s="4">
         <v>5</v>
       </c>
-      <c r="D50" s="4">
+      <c r="F50" s="4">
         <v>5</v>
       </c>
-      <c r="E50" s="4">
-        <v>4</v>
-      </c>
-      <c r="F50" s="4">
-        <v>4</v>
-      </c>
       <c r="G50" s="4">
         <v>4</v>
       </c>
       <c r="H50" s="4">
-        <v>3</v>
-      </c>
-      <c r="I50" s="3">
-        <v>1</v>
-      </c>
-      <c r="J50" s="4"/>
-      <c r="K50" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="I50" s="4">
+        <v>4</v>
+      </c>
+      <c r="J50" s="4">
+        <v>3</v>
+      </c>
+      <c r="K50" s="3">
+        <v>1</v>
+      </c>
       <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
-      <c r="N50" s="3"/>
-      <c r="O50" s="3"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
       <c r="P50" s="3"/>
       <c r="Q50" s="3"/>
       <c r="R50" s="3"/>
@@ -3525,8 +3793,10 @@
       <c r="X50" s="3"/>
       <c r="Y50" s="3"/>
       <c r="Z50" s="3"/>
-    </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA50" s="3"/>
+      <c r="AB50" s="3"/>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>22</v>
       </c>
@@ -3534,42 +3804,42 @@
         <v>70</v>
       </c>
       <c r="C51" s="4">
+        <v>70</v>
+      </c>
+      <c r="D51" s="4">
+        <v>70</v>
+      </c>
+      <c r="E51" s="4">
         <v>60</v>
       </c>
-      <c r="D51" s="4">
+      <c r="F51" s="4">
         <v>51</v>
       </c>
-      <c r="E51" s="4">
+      <c r="G51" s="4">
         <v>33</v>
       </c>
-      <c r="F51" s="4">
+      <c r="H51" s="4">
         <v>33</v>
       </c>
-      <c r="G51" s="4">
-        <v>21</v>
-      </c>
-      <c r="H51" s="4">
-        <v>21</v>
-      </c>
-      <c r="I51" s="3">
+      <c r="I51" s="4">
         <v>21</v>
       </c>
       <c r="J51" s="4">
         <v>21</v>
       </c>
       <c r="K51" s="3">
+        <v>21</v>
+      </c>
+      <c r="L51" s="4">
+        <v>21</v>
+      </c>
+      <c r="M51" s="3">
         <v>19</v>
       </c>
-      <c r="L51" s="4">
+      <c r="N51" s="4">
         <v>15</v>
       </c>
-      <c r="M51" s="4">
-        <v>11</v>
-      </c>
-      <c r="N51" s="3">
-        <v>11</v>
-      </c>
-      <c r="O51" s="3">
+      <c r="O51" s="4">
         <v>11</v>
       </c>
       <c r="P51" s="3">
@@ -3579,128 +3849,142 @@
         <v>11</v>
       </c>
       <c r="R51" s="3">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="S51" s="3">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="T51" s="3">
-        <v>1</v>
-      </c>
-      <c r="U51" s="3"/>
-      <c r="V51" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="U51" s="3">
+        <v>1</v>
+      </c>
+      <c r="V51" s="3">
+        <v>1</v>
+      </c>
       <c r="W51" s="3"/>
       <c r="X51" s="3"/>
       <c r="Y51" s="3"/>
       <c r="Z51" s="3"/>
-    </row>
-    <row r="52" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AA51" s="3"/>
+      <c r="AB51" s="3"/>
+    </row>
+    <row r="52" spans="1:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B52" s="15">
         <f>SUM(B8:B51)</f>
-        <v>3665</v>
+        <v>4300</v>
       </c>
       <c r="C52" s="15">
         <f>SUM(C8:C51)</f>
+        <v>3818</v>
+      </c>
+      <c r="D52" s="15">
+        <f>SUM(D8:D51)</f>
+        <v>3665</v>
+      </c>
+      <c r="E52" s="15">
+        <f>SUM(E8:E51)</f>
         <v>2748</v>
       </c>
-      <c r="D52" s="14">
-        <f>SUM(D8:D51)</f>
+      <c r="F52" s="14">
+        <f>SUM(F8:F51)</f>
         <v>2184</v>
       </c>
-      <c r="E52" s="5">
-        <f t="shared" ref="E52:Z52" si="0">SUM(E8:E51)</f>
+      <c r="G52" s="5">
+        <f t="shared" ref="G52:AB52" si="0">SUM(G8:G51)</f>
         <v>1641</v>
       </c>
-      <c r="F52" s="5">
+      <c r="H52" s="5">
         <f t="shared" si="0"/>
         <v>1105</v>
       </c>
-      <c r="G52" s="5">
+      <c r="I52" s="5">
         <f t="shared" si="0"/>
         <v>977</v>
       </c>
-      <c r="H52" s="5">
+      <c r="J52" s="5">
         <f t="shared" si="0"/>
         <v>827</v>
       </c>
-      <c r="I52" s="5">
+      <c r="K52" s="5">
         <f t="shared" si="0"/>
         <v>569</v>
       </c>
-      <c r="J52" s="5">
+      <c r="L52" s="5">
         <f t="shared" si="0"/>
         <v>454</v>
       </c>
-      <c r="K52" s="5">
+      <c r="M52" s="5">
         <f t="shared" si="0"/>
         <v>335</v>
       </c>
-      <c r="L52" s="5">
+      <c r="N52" s="5">
         <f t="shared" si="0"/>
         <v>277</v>
       </c>
-      <c r="M52" s="5">
+      <c r="O52" s="5">
         <f t="shared" si="0"/>
         <v>232</v>
       </c>
-      <c r="N52" s="5">
+      <c r="P52" s="5">
         <f t="shared" si="0"/>
         <v>199</v>
       </c>
-      <c r="O52" s="5">
+      <c r="Q52" s="5">
         <f t="shared" si="0"/>
         <v>182</v>
       </c>
-      <c r="P52" s="5">
+      <c r="R52" s="5">
         <f t="shared" si="0"/>
         <v>116</v>
       </c>
-      <c r="Q52" s="5">
+      <c r="S52" s="5">
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
-      <c r="R52" s="5">
+      <c r="T52" s="5">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="S52" s="5">
+      <c r="U52" s="5">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="T52" s="5">
+      <c r="V52" s="5">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="U52" s="5">
+      <c r="W52" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="V52" s="5">
+      <c r="X52" s="5">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="W52" s="5">
+      <c r="Y52" s="5">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="X52" s="5">
+      <c r="Z52" s="5">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="Y52" s="5">
+      <c r="AA52" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="Z52" s="5">
+      <c r="AB52" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:26" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="1:28" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="16" t="s">
         <v>49</v>
       </c>
@@ -3715,16 +3999,18 @@
       <c r="J54" s="17"/>
       <c r="K54" s="17"/>
       <c r="L54" s="17"/>
+      <c r="M54" s="17"/>
+      <c r="N54" s="17"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="0UKJnRdOKWvG1qENRNPV/WTK1k2UhrhiOC9RW+GuUIDhTtjNzA9e1/whwG4WV0Ikh35DMPYlit1yKl1dQNTSVQ==" saltValue="bmglVvZM73cxlp+rO5JGOw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="HsuC3kBsAWuZspULUukzdPajwPHeM1JAI5G0icG1XNza3X1uRpc4nGeHrqw4rVeaxfYqSZhJC8VYYbJLJuLsYg==" saltValue="RjUc+2Q0JZWlG++a/tlZcQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
-    <mergeCell ref="A54:L54"/>
+    <mergeCell ref="A54:N54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="47" orientation="landscape" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="D52:Z52" formulaRange="1"/>
+    <ignoredError sqref="E52:AB52 B52:C52" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>